<commit_message>
atualização do campo de texto
</commit_message>
<xml_diff>
--- a/bancodedados.xlsx
+++ b/bancodedados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,189 +473,34 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>+55 21 96907-8778</t>
+          <t>Daniel</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Fabrício</t>
+          <t>empty</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>manda agr n</t>
+          <t>empty</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>empty</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>+55 21 99192-0338</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Nova Iguaçu</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Daniel Ti</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Daniel</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Nova Iguaçu</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>TI Cisbaf</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>eita</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Nilton TI</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Nilton</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Obrigado Nilton, me diga qual é a sua unidade.</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>+55 21 98084-0869</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>KETTILY</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>CISBAF</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>empty</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>